<commit_message>
avances hasta mayo 2024
</commit_message>
<xml_diff>
--- a/data/respuestasCuestionario.xlsx
+++ b/data/respuestasCuestionario.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vicentetejero/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E196E9D0-A223-ED47-90A2-27251DD48026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9C3399-C673-F748-8463-052D823F1ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{71C25374-E814-9341-8EC5-5D3C49CF731F}"/>
+    <workbookView xWindow="500" yWindow="5200" windowWidth="28800" windowHeight="17500" xr2:uid="{71C25374-E814-9341-8EC5-5D3C49CF731F}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="glosario" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="150">
   <si>
     <t>accept_status</t>
   </si>
@@ -484,6 +484,9 @@
   </si>
   <si>
     <t>Tue Jun  4 13:37:13 2024</t>
+  </si>
+  <si>
+    <t>total_crt</t>
   </si>
 </sst>
 </file>
@@ -519,9 +522,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -858,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4A84E63-AFDB-4A47-8D98-362305244E7C}">
   <dimension ref="A1:AL15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AO4" sqref="AO4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -996,6 +998,9 @@
       <c r="AK1" t="s">
         <v>35</v>
       </c>
+      <c r="AL1" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -1008,7 +1013,7 @@
         <v>64</v>
       </c>
       <c r="F2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="G2">
         <v>20</v>
@@ -1102,6 +1107,9 @@
       </c>
       <c r="AK2" t="s">
         <v>79</v>
+      </c>
+      <c r="AL2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
@@ -1192,6 +1200,9 @@
       <c r="AK3">
         <v>3</v>
       </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -1296,6 +1307,9 @@
       <c r="AJ4" t="s">
         <v>50</v>
       </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -1308,7 +1322,7 @@
         <v>64</v>
       </c>
       <c r="F5">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="G5">
         <v>100</v>
@@ -1399,6 +1413,9 @@
       </c>
       <c r="AJ5" t="s">
         <v>50</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.2">
@@ -1412,7 +1429,7 @@
         <v>64</v>
       </c>
       <c r="F6">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="G6">
         <v>5</v>
@@ -1506,6 +1523,9 @@
       </c>
       <c r="AK6">
         <v>0.5</v>
+      </c>
+      <c r="AL6">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.2">
@@ -1620,6 +1640,9 @@
       <c r="AK7">
         <v>0</v>
       </c>
+      <c r="AL7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -1733,9 +1756,12 @@
       <c r="AK8">
         <v>0.7</v>
       </c>
+      <c r="AL8">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+      <c r="A9">
         <v>9</v>
       </c>
       <c r="J9">
@@ -1749,6 +1775,9 @@
       </c>
       <c r="U9" t="s">
         <v>47</v>
+      </c>
+      <c r="AL9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.2">
@@ -1768,7 +1797,7 @@
         <v>52</v>
       </c>
       <c r="F10">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="G10">
         <v>100</v>
@@ -1862,6 +1891,9 @@
       </c>
       <c r="AK10">
         <v>5</v>
+      </c>
+      <c r="AL10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.2">
@@ -1976,6 +2008,9 @@
       <c r="AK11" t="s">
         <v>68</v>
       </c>
+      <c r="AL11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -1994,7 +2029,7 @@
         <v>52</v>
       </c>
       <c r="F12">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="G12">
         <v>5</v>
@@ -2088,6 +2123,9 @@
       </c>
       <c r="AK12">
         <v>0.6</v>
+      </c>
+      <c r="AL12">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.2">
@@ -2202,6 +2240,9 @@
       <c r="AK13" t="s">
         <v>76</v>
       </c>
+      <c r="AL13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -2220,7 +2261,7 @@
         <v>52</v>
       </c>
       <c r="F14">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="G14">
         <v>5</v>
@@ -2312,11 +2353,11 @@
       <c r="AJ14" t="s">
         <v>50</v>
       </c>
-      <c r="AK14" t="s">
-        <v>49</v>
+      <c r="AK14">
+        <v>5</v>
       </c>
       <c r="AL14">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.2">
@@ -2428,11 +2469,11 @@
       <c r="AJ15" t="s">
         <v>60</v>
       </c>
-      <c r="AK15" t="s">
-        <v>48</v>
+      <c r="AK15">
+        <v>10</v>
       </c>
       <c r="AL15">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2445,7 +2486,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Graphs side by side with their responses
</commit_message>
<xml_diff>
--- a/data/respuestasCuestionario.xlsx
+++ b/data/respuestasCuestionario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vicentetejero/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9C3399-C673-F748-8463-052D823F1ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C2C04B-6603-8F49-8E45-9CADEE1A7D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="5200" windowWidth="28800" windowHeight="17500" xr2:uid="{71C25374-E814-9341-8EC5-5D3C49CF731F}"/>
+    <workbookView xWindow="-100" yWindow="5820" windowWidth="28800" windowHeight="17500" xr2:uid="{71C25374-E814-9341-8EC5-5D3C49CF731F}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="150">
   <si>
     <t>accept_status</t>
   </si>
@@ -860,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4A84E63-AFDB-4A47-8D98-362305244E7C}">
   <dimension ref="A1:AL15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AO4" sqref="AO4"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AK22" sqref="AK22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1764,20 +1764,110 @@
       <c r="A9">
         <v>9</v>
       </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>100</v>
+      </c>
+      <c r="H9">
+        <v>47</v>
+      </c>
       <c r="J9">
         <v>23</v>
       </c>
+      <c r="K9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L9" t="s">
+        <v>37</v>
+      </c>
+      <c r="M9" t="s">
+        <v>45</v>
+      </c>
       <c r="N9" t="s">
         <v>41</v>
       </c>
+      <c r="O9" t="s">
+        <v>75</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>56</v>
+      </c>
+      <c r="R9" t="s">
+        <v>57</v>
+      </c>
+      <c r="S9" t="s">
+        <v>45</v>
+      </c>
       <c r="T9" t="s">
         <v>46</v>
       </c>
       <c r="U9" t="s">
         <v>47</v>
       </c>
+      <c r="V9" t="s">
+        <v>48</v>
+      </c>
+      <c r="W9" t="s">
+        <v>48</v>
+      </c>
+      <c r="X9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>50</v>
+      </c>
       <c r="AL9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.2">

</xml_diff>